<commit_message>
Last runs consistent resolution
</commit_message>
<xml_diff>
--- a/final_results/cs_data_abm.xlsx
+++ b/final_results/cs_data_abm.xlsx
@@ -487,13 +487,13 @@
         <v>1</v>
       </c>
       <c r="F2" t="n">
-        <v>0.5400104978354978</v>
+        <v>0.1531268371546149</v>
       </c>
       <c r="G2" t="n">
-        <v>11.24695871212121</v>
+        <v>0.5341187720458554</v>
       </c>
       <c r="H2" t="n">
-        <v>21.028</v>
+        <v>2.073148148148148</v>
       </c>
     </row>
     <row r="3">
@@ -510,16 +510,16 @@
         <v>5</v>
       </c>
       <c r="E3" t="n">
-        <v>1.35593220338983</v>
+        <v>1.310344827586207</v>
       </c>
       <c r="F3" t="n">
-        <v>1.049256574522464</v>
+        <v>0.6425720956486043</v>
       </c>
       <c r="G3" t="n">
-        <v>10.82580962469734</v>
+        <v>1.147205972906404</v>
       </c>
       <c r="H3" t="n">
-        <v>20.47694915254237</v>
+        <v>3.752241379310345</v>
       </c>
     </row>
     <row r="4">
@@ -536,16 +536,16 @@
         <v>3</v>
       </c>
       <c r="E4" t="n">
-        <v>1.181818181818182</v>
+        <v>1.12280701754386</v>
       </c>
       <c r="F4" t="n">
-        <v>0.8624448953823954</v>
+        <v>0.405733761487051</v>
       </c>
       <c r="G4" t="n">
-        <v>11.8811136002886</v>
+        <v>1.123444688109162</v>
       </c>
       <c r="H4" t="n">
-        <v>22.30309090909091</v>
+        <v>3.481929824561404</v>
       </c>
     </row>
     <row r="5">
@@ -565,13 +565,13 @@
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>0.6387085912698413</v>
+        <v>0.2005680555555555</v>
       </c>
       <c r="G5" t="n">
-        <v>12.46610726190476</v>
+        <v>0.6531014770723105</v>
       </c>
       <c r="H5" t="n">
-        <v>23.2232</v>
+        <v>2.411333333333333</v>
       </c>
     </row>
     <row r="6">
@@ -588,16 +588,16 @@
         <v>5</v>
       </c>
       <c r="E6" t="n">
-        <v>1.428571428571429</v>
+        <v>1.388888888888889</v>
       </c>
       <c r="F6" t="n">
-        <v>1.091405108339632</v>
+        <v>0.7214347075249853</v>
       </c>
       <c r="G6" t="n">
-        <v>10.169242835097</v>
+        <v>1.679037716784245</v>
       </c>
       <c r="H6" t="n">
-        <v>19.23809523809524</v>
+        <v>4.601296296296296</v>
       </c>
     </row>
     <row r="7">
@@ -614,16 +614,16 @@
         <v>3</v>
       </c>
       <c r="E7" t="n">
-        <v>1.170212765957447</v>
+        <v>1.122448979591837</v>
       </c>
       <c r="F7" t="n">
-        <v>0.9095696977372508</v>
+        <v>0.4891171849692258</v>
       </c>
       <c r="G7" t="n">
-        <v>13.71426437436677</v>
+        <v>1.300359511661808</v>
       </c>
       <c r="H7" t="n">
-        <v>25.44723404255319</v>
+        <v>3.898979591836734</v>
       </c>
     </row>
     <row r="8">
@@ -643,13 +643,13 @@
         <v>1</v>
       </c>
       <c r="F8" t="n">
-        <v>0.4542899267399267</v>
+        <v>0.1155166761148904</v>
       </c>
       <c r="G8" t="n">
-        <v>9.12403701159951</v>
+        <v>0.7168164682539683</v>
       </c>
       <c r="H8" t="n">
-        <v>17.77753846153846</v>
+        <v>2.202380952380953</v>
       </c>
     </row>
     <row r="9">
@@ -666,16 +666,16 @@
         <v>5</v>
       </c>
       <c r="E9" t="n">
-        <v>1.194029850746269</v>
+        <v>1.1875</v>
       </c>
       <c r="F9" t="n">
-        <v>0.8163915837479272</v>
+        <v>0.5104406156994048</v>
       </c>
       <c r="G9" t="n">
-        <v>9.83486044479981</v>
+        <v>1.902392578125</v>
       </c>
       <c r="H9" t="n">
-        <v>18.71462686567164</v>
+        <v>5.13953125</v>
       </c>
     </row>
     <row r="10">
@@ -692,16 +692,16 @@
         <v>3</v>
       </c>
       <c r="E10" t="n">
-        <v>1.08695652173913</v>
+        <v>1.063492063492063</v>
       </c>
       <c r="F10" t="n">
-        <v>0.6345569933287325</v>
+        <v>0.3262371346686823</v>
       </c>
       <c r="G10" t="n">
-        <v>9.314728893489763</v>
+        <v>1.726775714915596</v>
       </c>
       <c r="H10" t="n">
-        <v>17.75666666666667</v>
+        <v>4.581904761904762</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Second to last runs
</commit_message>
<xml_diff>
--- a/final_results/cs_data_abm.xlsx
+++ b/final_results/cs_data_abm.xlsx
@@ -487,13 +487,13 @@
         <v>1</v>
       </c>
       <c r="F2" t="n">
-        <v>0.1531268371546149</v>
+        <v>0.2300463546529723</v>
       </c>
       <c r="G2" t="n">
-        <v>0.5341187720458554</v>
+        <v>1.47312266573296</v>
       </c>
       <c r="H2" t="n">
-        <v>2.073148148148148</v>
+        <v>4.175686274509804</v>
       </c>
     </row>
     <row r="3">
@@ -510,16 +510,16 @@
         <v>5</v>
       </c>
       <c r="E3" t="n">
-        <v>1.310344827586207</v>
+        <v>1.333333333333333</v>
       </c>
       <c r="F3" t="n">
-        <v>0.6425720956486043</v>
+        <v>0.9035628306878307</v>
       </c>
       <c r="G3" t="n">
-        <v>1.147205972906404</v>
+        <v>3.804974794238683</v>
       </c>
       <c r="H3" t="n">
-        <v>3.752241379310345</v>
+        <v>9.017962962962963</v>
       </c>
     </row>
     <row r="4">
@@ -536,16 +536,16 @@
         <v>3</v>
       </c>
       <c r="E4" t="n">
-        <v>1.12280701754386</v>
+        <v>1.132075471698113</v>
       </c>
       <c r="F4" t="n">
-        <v>0.405733761487051</v>
+        <v>0.6101235212638515</v>
       </c>
       <c r="G4" t="n">
-        <v>1.123444688109162</v>
+        <v>2.972091344713986</v>
       </c>
       <c r="H4" t="n">
-        <v>3.481929824561404</v>
+        <v>7.520754716981132</v>
       </c>
     </row>
     <row r="5">
@@ -565,13 +565,13 @@
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>0.2005680555555555</v>
+        <v>0.3143800329074719</v>
       </c>
       <c r="G5" t="n">
-        <v>0.6531014770723105</v>
+        <v>3.824024366047232</v>
       </c>
       <c r="H5" t="n">
-        <v>2.411333333333333</v>
+        <v>8.706829268292683</v>
       </c>
     </row>
     <row r="6">
@@ -588,16 +588,16 @@
         <v>5</v>
       </c>
       <c r="E6" t="n">
-        <v>1.388888888888889</v>
+        <v>1.428571428571429</v>
       </c>
       <c r="F6" t="n">
-        <v>0.7214347075249853</v>
+        <v>1.133932985098801</v>
       </c>
       <c r="G6" t="n">
-        <v>1.679037716784245</v>
+        <v>4.242640954000648</v>
       </c>
       <c r="H6" t="n">
-        <v>4.601296296296296</v>
+        <v>9.810204081632653</v>
       </c>
     </row>
     <row r="7">
@@ -614,16 +614,16 @@
         <v>3</v>
       </c>
       <c r="E7" t="n">
-        <v>1.122448979591837</v>
+        <v>1.209302325581395</v>
       </c>
       <c r="F7" t="n">
-        <v>0.4891171849692258</v>
+        <v>0.8171995893318567</v>
       </c>
       <c r="G7" t="n">
-        <v>1.300359511661808</v>
+        <v>4.336273301956441</v>
       </c>
       <c r="H7" t="n">
-        <v>3.898979591836734</v>
+        <v>9.983488372093023</v>
       </c>
     </row>
     <row r="8">
@@ -643,13 +643,13 @@
         <v>1</v>
       </c>
       <c r="F8" t="n">
-        <v>0.1155166761148904</v>
+        <v>0.1253704264191552</v>
       </c>
       <c r="G8" t="n">
-        <v>0.7168164682539683</v>
+        <v>0.5992779459241324</v>
       </c>
       <c r="H8" t="n">
-        <v>2.202380952380953</v>
+        <v>2.119322033898305</v>
       </c>
     </row>
     <row r="9">
@@ -666,16 +666,16 @@
         <v>5</v>
       </c>
       <c r="E9" t="n">
-        <v>1.1875</v>
+        <v>1.2</v>
       </c>
       <c r="F9" t="n">
-        <v>0.5104406156994048</v>
+        <v>0.5421815972222221</v>
       </c>
       <c r="G9" t="n">
-        <v>1.902392578125</v>
+        <v>2.041969113756613</v>
       </c>
       <c r="H9" t="n">
-        <v>5.13953125</v>
+        <v>5.497833333333333</v>
       </c>
     </row>
     <row r="10">
@@ -692,16 +692,16 @@
         <v>3</v>
       </c>
       <c r="E10" t="n">
-        <v>1.063492063492063</v>
+        <v>1.05</v>
       </c>
       <c r="F10" t="n">
-        <v>0.3262371346686823</v>
+        <v>0.3355795469576719</v>
       </c>
       <c r="G10" t="n">
-        <v>1.726775714915596</v>
+        <v>1.598878819444445</v>
       </c>
       <c r="H10" t="n">
-        <v>4.581904761904762</v>
+        <v>4.365166666666667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>